<commit_message>
"Updated App.tsx, ViewData.tsx, ViewDataGet.tsx, and hook.ts files with changes to data handling, Excel file export, and styling."
</commit_message>
<xml_diff>
--- a/public/example.xlsx
+++ b/public/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\react\read-bill\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AD22DC-EC72-4AED-97A6-88DB4BDB4096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BB542C-D148-4CC7-9C47-F999E2B50E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,35 +82,50 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -158,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -168,16 +183,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -185,6 +215,21 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -198,139 +243,62 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -343,19 +311,60 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -638,154 +647,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="14.25" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.9140625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="13.08203125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="8.9140625" style="32" customWidth="1"/>
-    <col min="5" max="5" width="11.9140625" style="32" customWidth="1"/>
-    <col min="6" max="6" width="8.9140625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="11.25" style="32" customWidth="1"/>
-    <col min="8" max="8" width="11.4140625" style="32" customWidth="1"/>
-    <col min="9" max="9" width="12" style="32" customWidth="1"/>
-    <col min="10" max="10" width="8.9140625" style="32" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="32"/>
-    <col min="12" max="16384" width="8.6640625" style="9"/>
+    <col min="1" max="1" width="19" style="7" customWidth="1"/>
+    <col min="2" max="2" width="16.08203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="20.25" style="7" customWidth="1"/>
+    <col min="4" max="4" width="19.25" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="11.08203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="16" style="7" customWidth="1"/>
+    <col min="9" max="9" width="16.75" style="7" customWidth="1"/>
+    <col min="10" max="10" width="15.08203125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="19" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="46.75" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.4" customHeight="1">
-      <c r="A2" s="1">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="15">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="16">
         <v>3</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="15">
         <v>4</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="15">
         <v>5</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="15">
         <v>6</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="15">
         <v>7</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="15">
         <v>8</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="17">
         <v>9</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="15">
         <v>10</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="15">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="17"/>
+    <row r="3" spans="1:11" ht="23" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
+    <row r="4" spans="1:11" s="6" customFormat="1" ht="14.4" customHeight="1" thickBot="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" s="29" customFormat="1" ht="14.4" customHeight="1">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+    <row r="5" spans="1:11">
+      <c r="A5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="19"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="31"/>
+      <c r="A6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="21"/>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="33"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="30" t="s">
+    <row r="7" spans="1:11" ht="14.5" thickBot="1">
+      <c r="A7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="34"/>
+      <c r="B7" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
"Updated App.tsx and App.css, and modified example.xlsx"
</commit_message>
<xml_diff>
--- a/public/example.xlsx
+++ b/public/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\react\read-bill\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BB542C-D148-4CC7-9C47-F999E2B50E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19482E0E-F4F4-493C-A29A-231B9F94199A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Ký hiệu hóa đơn</t>
   </si>
@@ -55,15 +55,6 @@
   </si>
   <si>
     <t>Tình trạng khách hàng mua</t>
-  </si>
-  <si>
-    <t>Nguồn tra cứu 1</t>
-  </si>
-  <si>
-    <t>Nguồn tra cứu 2</t>
-  </si>
-  <si>
-    <t>Đầu vào</t>
   </si>
   <si>
     <t>Time tra cứu</t>
@@ -73,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,13 +77,6 @@
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
@@ -173,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -196,101 +180,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -314,58 +208,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -647,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -701,7 +577,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.4" customHeight="1">
@@ -752,7 +628,7 @@
       <c r="J3" s="12"/>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:11" s="6" customFormat="1" ht="14.4" customHeight="1" thickBot="1">
+    <row r="4" spans="1:11" s="6" customFormat="1" ht="14.4" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -765,24 +641,6 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="19"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="21"/>
-    </row>
-    <row r="7" spans="1:11" ht="14.5" thickBot="1">
-      <c r="A7" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="23"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"Updated App.tsx and ViewDataGet.tsx files, moved covertCode function to common folder, and modified Excel file."
</commit_message>
<xml_diff>
--- a/public/example.xlsx
+++ b/public/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\react\read-bill\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19482E0E-F4F4-493C-A29A-231B9F94199A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862DABEB-32B7-4F9A-8880-70D4FAA0AB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Ký hiệu hóa đơn</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Time tra cứu</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
   </si>
 </sst>
 </file>
@@ -184,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -238,10 +241,6 @@
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,29 +522,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="19" style="7" customWidth="1"/>
-    <col min="2" max="2" width="16.08203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.25" style="7" customWidth="1"/>
-    <col min="4" max="4" width="19.25" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="11.08203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="16" style="7" customWidth="1"/>
-    <col min="9" max="9" width="16.75" style="7" customWidth="1"/>
-    <col min="10" max="10" width="15.08203125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="19" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="16.09765625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="20.19921875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="19.19921875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.69921875" style="7" customWidth="1"/>
+    <col min="6" max="7" width="17.69921875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="11.09765625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="16" style="7" customWidth="1"/>
+    <col min="10" max="10" width="16.69921875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="15.09765625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="19" style="7" customWidth="1"/>
+    <col min="13" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="46.75" customHeight="1">
+    <row r="1" spans="1:12" ht="46.8" customHeight="1">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -565,22 +564,25 @@
         <v>7</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.4" customHeight="1">
+    <row r="2" spans="1:12" ht="14.4" customHeight="1">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -605,7 +607,7 @@
       <c r="H2" s="15">
         <v>8</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="16">
         <v>9</v>
       </c>
       <c r="J2" s="15">
@@ -614,21 +616,25 @@
       <c r="K2" s="15">
         <v>11</v>
       </c>
+      <c r="L2" s="15">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="23" customHeight="1">
+    <row r="3" spans="1:12" ht="22.95" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="13"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:11" s="6" customFormat="1" ht="14.4" customHeight="1">
+    <row r="4" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -637,9 +643,10 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
"Updated index.html, App.tsx, ViewDataGet.tsx, and hook.ts files with changes to HTML structure, component rendering, and file upload functionality."
</commit_message>
<xml_diff>
--- a/public/example.xlsx
+++ b/public/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\react\read-bill\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862DABEB-32B7-4F9A-8880-70D4FAA0AB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB12167-D4D3-42D5-9FBD-3DC2072C82CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,15 +106,6 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -187,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -234,12 +225,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -522,29 +507,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="19" style="7" customWidth="1"/>
-    <col min="2" max="2" width="16.09765625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.19921875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="19.19921875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.69921875" style="7" customWidth="1"/>
-    <col min="6" max="7" width="17.69921875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="11.09765625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="16.08203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="7" customWidth="1"/>
+    <col min="6" max="7" width="17.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="11.08203125" style="7" customWidth="1"/>
     <col min="9" max="9" width="16" style="7" customWidth="1"/>
-    <col min="10" max="10" width="16.69921875" style="7" customWidth="1"/>
-    <col min="11" max="11" width="15.09765625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="15.08203125" style="7" customWidth="1"/>
     <col min="12" max="12" width="19" style="7" customWidth="1"/>
-    <col min="13" max="16384" width="8.69921875" style="1"/>
+    <col min="13" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="46.8" customHeight="1">
+    <row r="1" spans="1:12" ht="46.75" customHeight="1">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -582,71 +567,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="15">
-        <v>2</v>
-      </c>
-      <c r="C2" s="16">
-        <v>3</v>
-      </c>
-      <c r="D2" s="15">
-        <v>4</v>
-      </c>
-      <c r="E2" s="15">
-        <v>5</v>
-      </c>
-      <c r="F2" s="15">
-        <v>6</v>
-      </c>
-      <c r="G2" s="15">
-        <v>7</v>
-      </c>
-      <c r="H2" s="15">
-        <v>8</v>
-      </c>
-      <c r="I2" s="16">
-        <v>9</v>
-      </c>
-      <c r="J2" s="15">
-        <v>10</v>
-      </c>
-      <c r="K2" s="15">
-        <v>11</v>
-      </c>
-      <c r="L2" s="15">
-        <v>12</v>
-      </c>
+    <row r="2" spans="1:12" ht="23" customHeight="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:12" ht="22.95" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
-    </row>
-    <row r="4" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+    <row r="3" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>